<commit_message>
build based on 0294d82
</commit_message>
<xml_diff>
--- a/dev/examples/results/output_file_ANC.xlsx
+++ b/dev/examples/results/output_file_ANC.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>comp_time</t>
   </si>
@@ -113,9 +113,6 @@
     <t>x_us_PV</t>
   </si>
   <si>
-    <t>x_us_generator</t>
-  </si>
-  <si>
     <t>x_us_batt</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>CAPEX_us_PV</t>
   </si>
   <si>
-    <t>CAPEX_us_generator</t>
-  </si>
-  <si>
     <t>CAPEX_us_batt</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
   </si>
   <si>
     <t>C_OEM_us_PV</t>
-  </si>
-  <si>
-    <t>C_OEM_us_generator</t>
   </si>
   <si>
     <t>C_OEM_us_batt</t>
@@ -565,7 +556,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>2.006768226623535</v>
+        <v>1.3108773231506348</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -606,22 +597,22 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>8570.26245186916</v>
+        <v>8530.582818480752</v>
       </c>
       <c r="B2">
         <v>-56242.6959069909</v>
       </c>
       <c r="C2">
-        <v>8570.26245186916</v>
+        <v>8530.582818480752</v>
       </c>
       <c r="D2">
-        <v>-1.214171631691499e6</v>
+        <v>-1.2142113113248872e6</v>
       </c>
       <c r="E2">
-        <v>-1.2227418941433681e6</v>
+        <v>-1.222741894143368e6</v>
       </c>
       <c r="F2">
-        <v>576.0562549931785</v>
+        <v>573.3891603577929</v>
       </c>
     </row>
   </sheetData>
@@ -683,10 +674,10 @@
         <v>21</v>
       </c>
       <c r="B2">
-        <v>74.95440187624375</v>
+        <v>74.95619728130688</v>
       </c>
       <c r="C2">
-        <v>103.67293866601536</v>
+        <v>103.67293866601534</v>
       </c>
       <c r="D2">
         <v>83.60487675774463</v>
@@ -695,25 +686,25 @@
         <v>78.37325772970166</v>
       </c>
       <c r="F2">
-        <v>66.08642737631462</v>
+        <v>63.832102472583365</v>
       </c>
       <c r="G2">
-        <v>71.09777497045127</v>
+        <v>71.09777497045125</v>
       </c>
       <c r="H2">
-        <v>83.6157224188135</v>
+        <v>83.61572241881349</v>
       </c>
       <c r="I2">
-        <v>75.55808313800487</v>
+        <v>75.55808313800486</v>
       </c>
       <c r="J2">
-        <v>72.45316041995376</v>
+        <v>71.05252151118073</v>
       </c>
       <c r="K2">
-        <v>68.78135473909617</v>
+        <v>67.73624642560675</v>
       </c>
       <c r="L2">
-        <v>78.81711346915317</v>
+        <v>78.81711346915316</v>
       </c>
       <c r="M2">
         <v>97.6114955735004</v>
@@ -726,13 +717,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -757,13 +748,10 @@
       <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>31</v>
       </c>
       <c r="B2">
         <v>55.29324587</v>
@@ -775,16 +763,13 @@
       <c r="E2">
         <v>50.0</v>
       </c>
-      <c r="F2">
-        <v>0.0</v>
-      </c>
+      <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
-      <c r="I2"/>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>27.00540954</v>
@@ -796,18 +781,17 @@
       <c r="E3">
         <v>25.489185845443384</v>
       </c>
-      <c r="F3"/>
+      <c r="F3">
+        <v>1.973245920368238</v>
+      </c>
       <c r="G3">
         <v>1.973245920368238</v>
       </c>
-      <c r="H3">
-        <v>1.973245920368238</v>
-      </c>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>45.40292054</v>
@@ -817,17 +801,16 @@
       </c>
       <c r="D4"/>
       <c r="E4">
-        <v>44.04652629600476</v>
-      </c>
-      <c r="F4"/>
+        <v>44.04652629600474</v>
+      </c>
+      <c r="F4">
+        <v>3.7213684553918602</v>
+      </c>
       <c r="G4">
-        <v>3.721368455391854</v>
+        <v>3.7213684553918602</v>
       </c>
       <c r="H4">
-        <v>3.721368455391854</v>
-      </c>
-      <c r="I4">
-        <v>34.906983718279776</v>
+        <v>34.906983718279804</v>
       </c>
     </row>
   </sheetData>
@@ -837,83 +820,77 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>40</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>41</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>42</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>46</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>47</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>48</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>50</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>51</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>52</v>
       </c>
-      <c r="T1" t="s">
-        <v>53</v>
-      </c>
-      <c r="U1" t="s">
-        <v>54</v>
-      </c>
-      <c r="V1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>-563669.0832118867</v>
@@ -925,7 +902,7 @@
         <v>-31580.287385073458</v>
       </c>
       <c r="E2">
-        <v>-8.573955168024072e-14</v>
+        <v>0.0</v>
       </c>
       <c r="F2">
         <v>22316.212290683256</v>
@@ -946,35 +923,29 @@
       <c r="L2">
         <v>85000.0</v>
       </c>
-      <c r="M2">
-        <v>0.0</v>
-      </c>
+      <c r="M2"/>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2">
+      <c r="Q2">
         <v>1500.0</v>
       </c>
-      <c r="S2">
-        <v>0.0</v>
-      </c>
+      <c r="R2"/>
+      <c r="S2"/>
       <c r="T2"/>
-      <c r="U2"/>
-      <c r="V2"/>
-    </row>
-    <row r="3" spans="1:22">
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
-        <v>-223241.12057109879</v>
+        <v>-223241.12057109867</v>
       </c>
       <c r="C3">
         <v>36868.807735841685</v>
       </c>
       <c r="D3">
-        <v>-12164.328747674768</v>
+        <v>-12164.328747674772</v>
       </c>
       <c r="E3">
         <v>0.0</v>
@@ -992,91 +963,87 @@
         <v>8840.453007913167</v>
       </c>
       <c r="J3">
-        <v>-169392.55507295928</v>
+        <v>-169392.5550729593</v>
       </c>
       <c r="K3"/>
       <c r="L3">
         <v>35684.86018362074</v>
       </c>
-      <c r="M3"/>
+      <c r="M3">
+        <v>789.2983681472952</v>
+      </c>
       <c r="N3">
-        <v>789.2983681472952</v>
-      </c>
-      <c r="O3">
         <v>394.6491840736476</v>
       </c>
+      <c r="O3"/>
       <c r="P3"/>
-      <c r="Q3"/>
+      <c r="Q3">
+        <v>764.6755753633015</v>
+      </c>
       <c r="R3">
-        <v>764.6755753633015</v>
-      </c>
-      <c r="S3"/>
-      <c r="T3">
         <v>9.86622960184119</v>
       </c>
-      <c r="U3">
+      <c r="S3">
         <v>3.946491840736476</v>
       </c>
-      <c r="V3"/>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="T3"/>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>-435831.69036038255</v>
       </c>
       <c r="C4">
-        <v>177428.21430168205</v>
+        <v>177428.2143016821</v>
       </c>
       <c r="D4">
-        <v>-17171.222950664833</v>
+        <v>-17171.222950664825</v>
       </c>
       <c r="E4">
         <v>0.0</v>
       </c>
       <c r="F4">
-        <v>35626.41777095829</v>
+        <v>35626.4177709583</v>
       </c>
       <c r="G4">
-        <v>1509.2514460525526</v>
+        <v>1509.251446052555</v>
       </c>
       <c r="H4">
         <v>8353.446369498317</v>
       </c>
       <c r="I4">
-        <v>9783.233210352739</v>
+        <v>9783.233210352735</v>
       </c>
       <c r="J4">
-        <v>-219838.02000083437</v>
+        <v>-219838.02000083425</v>
       </c>
       <c r="K4"/>
       <c r="L4">
-        <v>70474.44207360761</v>
-      </c>
-      <c r="M4"/>
+        <v>70474.44207360758</v>
+      </c>
+      <c r="M4">
+        <v>1488.547382156744</v>
+      </c>
       <c r="N4">
-        <v>1488.5473821567416</v>
+        <v>744.273691078372</v>
       </c>
       <c r="O4">
-        <v>744.2736910783708</v>
-      </c>
-      <c r="P4">
-        <v>104720.95115483932</v>
-      </c>
-      <c r="Q4"/>
+        <v>104720.95115483941</v>
+      </c>
+      <c r="P4"/>
+      <c r="Q4">
+        <v>1321.3957888801424</v>
+      </c>
       <c r="R4">
-        <v>1321.3957888801426</v>
-      </c>
-      <c r="S4"/>
+        <v>18.606842276959302</v>
+      </c>
+      <c r="S4">
+        <v>7.4427369107837205</v>
+      </c>
       <c r="T4">
-        <v>18.60684227695927</v>
-      </c>
-      <c r="U4">
-        <v>7.442736910783708</v>
-      </c>
-      <c r="V4">
-        <v>1047.2095115483933</v>
+        <v>1047.2095115483942</v>
       </c>
     </row>
   </sheetData>
@@ -1094,7 +1061,7 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -1135,7 +1102,7 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>50.3983545</v>
@@ -1177,7 +1144,7 @@
         <v>23.93422539963176</v>
       </c>
       <c r="O2">
-        <v>32.8611392682314</v>
+        <v>32.86113926823138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
build based on 7a80c9b
</commit_message>
<xml_diff>
--- a/dev/examples/results/output_file_ANC.xlsx
+++ b/dev/examples/results/output_file_ANC.xlsx
@@ -556,7 +556,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>1.297701120376587</v>
+        <v>1.3165929317474365</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -754,10 +754,10 @@
         <v>30</v>
       </c>
       <c r="B2">
-        <v>55.29324587</v>
+        <v>30523.270014740006</v>
       </c>
       <c r="C2">
-        <v>232.10403242918818</v>
+        <v>232.10403242918812</v>
       </c>
       <c r="D2"/>
       <c r="E2">
@@ -772,10 +772,10 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>27.00540954</v>
+        <v>12160.103553284996</v>
       </c>
       <c r="C3">
-        <v>92.46745411323812</v>
+        <v>92.467454113238</v>
       </c>
       <c r="D3"/>
       <c r="E3">
@@ -794,10 +794,10 @@
         <v>32</v>
       </c>
       <c r="B4">
-        <v>45.40292054</v>
+        <v>24500.351344201987</v>
       </c>
       <c r="C4">
-        <v>186.3047550336197</v>
+        <v>186.30475503361959</v>
       </c>
       <c r="D4"/>
       <c r="E4">

</xml_diff>

<commit_message>
build based on f59c2fd
</commit_message>
<xml_diff>
--- a/dev/examples/results/output_file_ANC.xlsx
+++ b/dev/examples/results/output_file_ANC.xlsx
@@ -556,7 +556,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>1.3211989402770996</v>
+        <v>1.330852746963501</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -939,7 +939,7 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>-223241.12057109867</v>
+        <v>-223241.1205710986</v>
       </c>
       <c r="C3">
         <v>36868.807735841685</v>
@@ -954,7 +954,7 @@
         <v>11581.94006488829</v>
       </c>
       <c r="G3">
-        <v>800.2766440442327</v>
+        <v>800.2766440442326</v>
       </c>
       <c r="H3">
         <v>4242.911954548019</v>

</xml_diff>